<commit_message>
Add padding byte in bl hash to fit flasher script
</commit_message>
<xml_diff>
--- a/docs/dfu/DFU packets.xlsx
+++ b/docs/dfu/DFU packets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18720" windowHeight="12225" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18720" windowHeight="12225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Memory map" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="273">
   <si>
     <t>Handle</t>
   </si>
@@ -842,6 +842,12 @@
   </si>
   <si>
     <t>NOT IMPLEMENTED</t>
+  </si>
+  <si>
+    <t>Padding</t>
+  </si>
+  <si>
+    <t>Single byte padding to fit format in nrfutil-script</t>
   </si>
 </sst>
 </file>
@@ -1796,6 +1802,160 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1805,39 +1965,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1847,126 +1977,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1992,12 +2040,6 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2016,39 +2058,6 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2066,9 +2075,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3955,7 +3961,7 @@
   </sheetPr>
   <dimension ref="B2:BM218"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AY12" sqref="AY12"/>
     </sheetView>
   </sheetViews>
@@ -4114,87 +4120,87 @@
       <c r="AV3" s="11">
         <v>46</v>
       </c>
-      <c r="AY3" s="153" t="s">
+      <c r="AY3" s="136" t="s">
         <v>243</v>
       </c>
-      <c r="AZ3" s="154"/>
-      <c r="BA3" s="154"/>
-      <c r="BB3" s="154"/>
-      <c r="BC3" s="154"/>
-      <c r="BD3" s="154"/>
-      <c r="BE3" s="154"/>
-      <c r="BF3" s="155"/>
+      <c r="AZ3" s="137"/>
+      <c r="BA3" s="137"/>
+      <c r="BB3" s="137"/>
+      <c r="BC3" s="137"/>
+      <c r="BD3" s="137"/>
+      <c r="BE3" s="137"/>
+      <c r="BF3" s="138"/>
     </row>
     <row r="4" spans="2:60" s="46" customFormat="1" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="149" t="s">
+      <c r="C4" s="157" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="150"/>
-      <c r="E4" s="150"/>
-      <c r="F4" s="151"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="158"/>
       <c r="G4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="149" t="s">
+      <c r="I4" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="150"/>
-      <c r="K4" s="150"/>
-      <c r="L4" s="150"/>
-      <c r="M4" s="150"/>
-      <c r="N4" s="151"/>
+      <c r="J4" s="144"/>
+      <c r="K4" s="144"/>
+      <c r="L4" s="144"/>
+      <c r="M4" s="144"/>
+      <c r="N4" s="158"/>
       <c r="O4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="152" t="s">
+      <c r="Q4" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="152"/>
-      <c r="S4" s="135" t="s">
+      <c r="R4" s="159"/>
+      <c r="S4" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="T4" s="144"/>
-      <c r="U4" s="145" t="s">
+      <c r="T4" s="146"/>
+      <c r="U4" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="V4" s="116"/>
-      <c r="W4" s="116"/>
-      <c r="X4" s="116"/>
-      <c r="Y4" s="116"/>
-      <c r="Z4" s="116"/>
-      <c r="AA4" s="116"/>
-      <c r="AB4" s="116"/>
-      <c r="AC4" s="116"/>
-      <c r="AD4" s="116"/>
-      <c r="AE4" s="116"/>
-      <c r="AF4" s="116"/>
-      <c r="AG4" s="116"/>
-      <c r="AH4" s="116"/>
-      <c r="AI4" s="116"/>
-      <c r="AJ4" s="116"/>
-      <c r="AK4" s="116"/>
-      <c r="AL4" s="116"/>
-      <c r="AM4" s="116"/>
-      <c r="AN4" s="116"/>
-      <c r="AO4" s="116"/>
-      <c r="AP4" s="116"/>
-      <c r="AQ4" s="116"/>
-      <c r="AR4" s="116"/>
-      <c r="AS4" s="119"/>
-      <c r="AT4" s="159" t="s">
+      <c r="V4" s="119"/>
+      <c r="W4" s="119"/>
+      <c r="X4" s="119"/>
+      <c r="Y4" s="119"/>
+      <c r="Z4" s="119"/>
+      <c r="AA4" s="119"/>
+      <c r="AB4" s="119"/>
+      <c r="AC4" s="119"/>
+      <c r="AD4" s="119"/>
+      <c r="AE4" s="119"/>
+      <c r="AF4" s="119"/>
+      <c r="AG4" s="119"/>
+      <c r="AH4" s="119"/>
+      <c r="AI4" s="119"/>
+      <c r="AJ4" s="119"/>
+      <c r="AK4" s="119"/>
+      <c r="AL4" s="119"/>
+      <c r="AM4" s="119"/>
+      <c r="AN4" s="119"/>
+      <c r="AO4" s="119"/>
+      <c r="AP4" s="119"/>
+      <c r="AQ4" s="119"/>
+      <c r="AR4" s="119"/>
+      <c r="AS4" s="120"/>
+      <c r="AT4" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="AU4" s="150"/>
-      <c r="AV4" s="160"/>
+      <c r="AU4" s="144"/>
+      <c r="AV4" s="145"/>
     </row>
     <row r="5" spans="2:60" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="S5" s="70"/>
@@ -4335,40 +4341,40 @@
       <c r="R8" s="71" t="s">
         <v>227</v>
       </c>
-      <c r="S8" s="135" t="s">
+      <c r="S8" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="144"/>
-      <c r="U8" s="145" t="s">
+      <c r="T8" s="146"/>
+      <c r="U8" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="V8" s="116"/>
-      <c r="W8" s="116"/>
-      <c r="X8" s="116"/>
-      <c r="Y8" s="116"/>
-      <c r="Z8" s="116"/>
-      <c r="AA8" s="116"/>
-      <c r="AB8" s="116"/>
-      <c r="AC8" s="116"/>
-      <c r="AD8" s="116"/>
-      <c r="AE8" s="116"/>
-      <c r="AF8" s="116"/>
-      <c r="AG8" s="116"/>
-      <c r="AH8" s="116"/>
-      <c r="AI8" s="116"/>
-      <c r="AJ8" s="116"/>
-      <c r="AK8" s="116"/>
-      <c r="AL8" s="116"/>
-      <c r="AM8" s="116"/>
-      <c r="AN8" s="116"/>
-      <c r="AO8" s="116"/>
-      <c r="AP8" s="116"/>
-      <c r="AQ8" s="116"/>
-      <c r="AR8" s="116"/>
-      <c r="AS8" s="119"/>
-      <c r="AT8" s="142"/>
-      <c r="AU8" s="143"/>
-      <c r="AV8" s="143"/>
+      <c r="V8" s="119"/>
+      <c r="W8" s="119"/>
+      <c r="X8" s="119"/>
+      <c r="Y8" s="119"/>
+      <c r="Z8" s="119"/>
+      <c r="AA8" s="119"/>
+      <c r="AB8" s="119"/>
+      <c r="AC8" s="119"/>
+      <c r="AD8" s="119"/>
+      <c r="AE8" s="119"/>
+      <c r="AF8" s="119"/>
+      <c r="AG8" s="119"/>
+      <c r="AH8" s="119"/>
+      <c r="AI8" s="119"/>
+      <c r="AJ8" s="119"/>
+      <c r="AK8" s="119"/>
+      <c r="AL8" s="119"/>
+      <c r="AM8" s="119"/>
+      <c r="AN8" s="119"/>
+      <c r="AO8" s="119"/>
+      <c r="AP8" s="119"/>
+      <c r="AQ8" s="119"/>
+      <c r="AR8" s="119"/>
+      <c r="AS8" s="120"/>
+      <c r="AT8" s="148"/>
+      <c r="AU8" s="149"/>
+      <c r="AV8" s="149"/>
     </row>
     <row r="9" spans="2:60" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="S9" s="70"/>
@@ -4509,40 +4515,40 @@
       <c r="R12" s="75" t="s">
         <v>227</v>
       </c>
-      <c r="S12" s="144" t="s">
+      <c r="S12" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="T12" s="144"/>
-      <c r="U12" s="145" t="s">
+      <c r="T12" s="146"/>
+      <c r="U12" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="V12" s="116"/>
-      <c r="W12" s="116"/>
-      <c r="X12" s="116"/>
-      <c r="Y12" s="116"/>
-      <c r="Z12" s="116"/>
-      <c r="AA12" s="116"/>
-      <c r="AB12" s="116"/>
-      <c r="AC12" s="116"/>
-      <c r="AD12" s="116"/>
-      <c r="AE12" s="116"/>
-      <c r="AF12" s="116"/>
-      <c r="AG12" s="116"/>
-      <c r="AH12" s="116"/>
-      <c r="AI12" s="116"/>
-      <c r="AJ12" s="116"/>
-      <c r="AK12" s="116"/>
-      <c r="AL12" s="116"/>
-      <c r="AM12" s="116"/>
-      <c r="AN12" s="116"/>
-      <c r="AO12" s="116"/>
-      <c r="AP12" s="116"/>
-      <c r="AQ12" s="116"/>
-      <c r="AR12" s="116"/>
-      <c r="AS12" s="119"/>
-      <c r="AT12" s="142"/>
-      <c r="AU12" s="143"/>
-      <c r="AV12" s="143"/>
+      <c r="V12" s="119"/>
+      <c r="W12" s="119"/>
+      <c r="X12" s="119"/>
+      <c r="Y12" s="119"/>
+      <c r="Z12" s="119"/>
+      <c r="AA12" s="119"/>
+      <c r="AB12" s="119"/>
+      <c r="AC12" s="119"/>
+      <c r="AD12" s="119"/>
+      <c r="AE12" s="119"/>
+      <c r="AF12" s="119"/>
+      <c r="AG12" s="119"/>
+      <c r="AH12" s="119"/>
+      <c r="AI12" s="119"/>
+      <c r="AJ12" s="119"/>
+      <c r="AK12" s="119"/>
+      <c r="AL12" s="119"/>
+      <c r="AM12" s="119"/>
+      <c r="AN12" s="119"/>
+      <c r="AO12" s="119"/>
+      <c r="AP12" s="119"/>
+      <c r="AQ12" s="119"/>
+      <c r="AR12" s="119"/>
+      <c r="AS12" s="120"/>
+      <c r="AT12" s="148"/>
+      <c r="AU12" s="149"/>
+      <c r="AV12" s="149"/>
       <c r="AY12" s="5" t="s">
         <v>229</v>
       </c>
@@ -4627,49 +4633,49 @@
       <c r="AU14" s="11"/>
     </row>
     <row r="15" spans="2:60" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J15" s="163" t="s">
+      <c r="J15" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="K15" s="164"/>
-      <c r="L15" s="164"/>
-      <c r="M15" s="164"/>
-      <c r="N15" s="137" t="s">
+      <c r="K15" s="151"/>
+      <c r="L15" s="151"/>
+      <c r="M15" s="151"/>
+      <c r="N15" s="131" t="s">
         <v>14</v>
       </c>
-      <c r="O15" s="137"/>
-      <c r="P15" s="137"/>
-      <c r="Q15" s="137"/>
-      <c r="R15" s="137"/>
-      <c r="S15" s="135" t="s">
+      <c r="O15" s="131"/>
+      <c r="P15" s="131"/>
+      <c r="Q15" s="131"/>
+      <c r="R15" s="131"/>
+      <c r="S15" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="T15" s="136"/>
-      <c r="U15" s="120" t="s">
+      <c r="T15" s="133"/>
+      <c r="U15" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="V15" s="148"/>
+      <c r="V15" s="163"/>
       <c r="W15" s="101" t="s">
         <v>268</v>
       </c>
       <c r="X15" s="100" t="s">
         <v>269</v>
       </c>
-      <c r="Y15" s="146" t="s">
+      <c r="Y15" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="Z15" s="146"/>
-      <c r="AA15" s="146"/>
-      <c r="AB15" s="147"/>
+      <c r="Z15" s="160"/>
+      <c r="AA15" s="160"/>
+      <c r="AB15" s="161"/>
       <c r="AC15" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="AD15" s="116"/>
+      <c r="AD15" s="119"/>
       <c r="AE15" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="AF15" s="116"/>
-      <c r="AG15" s="116"/>
-      <c r="AH15" s="119"/>
+      <c r="AF15" s="119"/>
+      <c r="AG15" s="119"/>
+      <c r="AH15" s="120"/>
       <c r="AI15" s="7"/>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="6"/>
@@ -4687,11 +4693,11 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="138"/>
-      <c r="O16" s="138"/>
-      <c r="P16" s="138"/>
-      <c r="Q16" s="138"/>
-      <c r="R16" s="138"/>
+      <c r="N16" s="124"/>
+      <c r="O16" s="124"/>
+      <c r="P16" s="124"/>
+      <c r="Q16" s="124"/>
+      <c r="R16" s="124"/>
       <c r="S16" s="24"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
@@ -4738,11 +4744,11 @@
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
-      <c r="N17" s="139"/>
-      <c r="O17" s="139"/>
-      <c r="P17" s="139"/>
-      <c r="Q17" s="139"/>
-      <c r="R17" s="139"/>
+      <c r="N17" s="130"/>
+      <c r="O17" s="130"/>
+      <c r="P17" s="130"/>
+      <c r="Q17" s="130"/>
+      <c r="R17" s="130"/>
       <c r="S17" s="78">
         <v>0</v>
       </c>
@@ -4835,51 +4841,51 @@
       <c r="BH17" s="79"/>
     </row>
     <row r="18" spans="5:63" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J18" s="161" t="s">
+      <c r="J18" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="162"/>
-      <c r="L18" s="162"/>
-      <c r="M18" s="162"/>
-      <c r="N18" s="137" t="s">
+      <c r="K18" s="114"/>
+      <c r="L18" s="114"/>
+      <c r="M18" s="114"/>
+      <c r="N18" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="137"/>
-      <c r="P18" s="137"/>
-      <c r="Q18" s="137"/>
-      <c r="R18" s="137"/>
-      <c r="S18" s="135" t="s">
+      <c r="O18" s="131"/>
+      <c r="P18" s="131"/>
+      <c r="Q18" s="131"/>
+      <c r="R18" s="131"/>
+      <c r="S18" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="T18" s="136"/>
+      <c r="T18" s="133"/>
       <c r="U18" s="85" t="s">
         <v>156</v>
       </c>
       <c r="V18" s="84" t="s">
         <v>231</v>
       </c>
-      <c r="W18" s="130" t="s">
+      <c r="W18" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="X18" s="131"/>
-      <c r="Y18" s="131"/>
-      <c r="Z18" s="132"/>
-      <c r="AA18" s="116" t="s">
+      <c r="X18" s="128"/>
+      <c r="Y18" s="128"/>
+      <c r="Z18" s="135"/>
+      <c r="AA18" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="AB18" s="116"/>
-      <c r="AC18" s="116"/>
-      <c r="AD18" s="117"/>
+      <c r="AB18" s="119"/>
+      <c r="AC18" s="119"/>
+      <c r="AD18" s="156"/>
       <c r="AE18" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="AF18" s="116"/>
+      <c r="AF18" s="119"/>
       <c r="AG18" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="AH18" s="116"/>
-      <c r="AI18" s="116"/>
-      <c r="AJ18" s="119"/>
+      <c r="AH18" s="119"/>
+      <c r="AI18" s="119"/>
+      <c r="AJ18" s="120"/>
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
       <c r="AM18" s="4"/>
@@ -4890,10 +4896,10 @@
       <c r="AU18" s="4"/>
       <c r="AV18" s="4"/>
       <c r="AW18" s="25"/>
-      <c r="AX18" s="165" t="s">
+      <c r="AX18" s="152" t="s">
         <v>156</v>
       </c>
-      <c r="AY18" s="166"/>
+      <c r="AY18" s="153"/>
       <c r="AZ18" s="13" t="s">
         <v>153</v>
       </c>
@@ -4906,19 +4912,19 @@
       <c r="BC18" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="BD18" s="167" t="s">
+      <c r="BD18" s="121" t="s">
         <v>249</v>
       </c>
-      <c r="BE18" s="168"/>
-      <c r="BF18" s="168"/>
-      <c r="BG18" s="169"/>
+      <c r="BE18" s="122"/>
+      <c r="BF18" s="122"/>
+      <c r="BG18" s="123"/>
       <c r="BH18" s="25"/>
     </row>
     <row r="19" spans="5:63" x14ac:dyDescent="0.25">
-      <c r="J19" s="161"/>
-      <c r="K19" s="162"/>
-      <c r="L19" s="162"/>
-      <c r="M19" s="162"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="114"/>
+      <c r="L19" s="114"/>
+      <c r="M19" s="114"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -4964,15 +4970,15 @@
       <c r="BH19" s="25"/>
     </row>
     <row r="20" spans="5:63" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J20" s="161"/>
-      <c r="K20" s="162"/>
-      <c r="L20" s="162"/>
-      <c r="M20" s="162"/>
-      <c r="N20" s="139"/>
-      <c r="O20" s="139"/>
-      <c r="P20" s="139"/>
-      <c r="Q20" s="139"/>
-      <c r="R20" s="139"/>
+      <c r="J20" s="113"/>
+      <c r="K20" s="114"/>
+      <c r="L20" s="114"/>
+      <c r="M20" s="114"/>
+      <c r="N20" s="130"/>
+      <c r="O20" s="130"/>
+      <c r="P20" s="130"/>
+      <c r="Q20" s="130"/>
+      <c r="R20" s="130"/>
       <c r="S20" s="78">
         <v>0</v>
       </c>
@@ -5051,37 +5057,37 @@
       <c r="BJ20" s="11"/>
     </row>
     <row r="21" spans="5:63" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J21" s="161"/>
-      <c r="K21" s="162"/>
-      <c r="L21" s="162"/>
-      <c r="M21" s="162"/>
-      <c r="N21" s="137" t="s">
+      <c r="J21" s="113"/>
+      <c r="K21" s="114"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="114"/>
+      <c r="N21" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="O21" s="137"/>
-      <c r="P21" s="137"/>
-      <c r="Q21" s="137"/>
-      <c r="R21" s="137"/>
-      <c r="S21" s="135" t="s">
+      <c r="O21" s="131"/>
+      <c r="P21" s="131"/>
+      <c r="Q21" s="131"/>
+      <c r="R21" s="131"/>
+      <c r="S21" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="T21" s="136"/>
+      <c r="T21" s="133"/>
       <c r="U21" s="85" t="s">
         <v>156</v>
       </c>
       <c r="V21" s="84" t="s">
         <v>231</v>
       </c>
-      <c r="W21" s="130" t="s">
+      <c r="W21" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="X21" s="131"/>
-      <c r="Y21" s="131"/>
-      <c r="Z21" s="132"/>
-      <c r="AA21" s="120" t="s">
+      <c r="X21" s="128"/>
+      <c r="Y21" s="128"/>
+      <c r="Z21" s="135"/>
+      <c r="AA21" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="AB21" s="121"/>
+      <c r="AB21" s="168"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
       <c r="AE21" s="4"/>
@@ -5098,36 +5104,36 @@
       <c r="AS21" s="25"/>
       <c r="AT21" s="14"/>
       <c r="AU21" s="12"/>
-      <c r="AX21" s="122" t="s">
+      <c r="AX21" s="154" t="s">
         <v>231</v>
       </c>
-      <c r="AY21" s="123"/>
-      <c r="AZ21" s="127" t="s">
+      <c r="AY21" s="155"/>
+      <c r="AZ21" s="169" t="s">
         <v>232</v>
       </c>
-      <c r="BA21" s="128"/>
-      <c r="BB21" s="129"/>
+      <c r="BA21" s="170"/>
+      <c r="BB21" s="171"/>
       <c r="BC21" s="13" t="s">
         <v>248</v>
       </c>
       <c r="BD21" s="98" t="s">
         <v>250</v>
       </c>
-      <c r="BE21" s="124" t="s">
+      <c r="BE21" s="115" t="s">
         <v>249</v>
       </c>
-      <c r="BF21" s="125"/>
-      <c r="BG21" s="126"/>
+      <c r="BF21" s="116"/>
+      <c r="BG21" s="117"/>
       <c r="BH21" s="29"/>
       <c r="BI21" s="31"/>
       <c r="BJ21" s="30"/>
       <c r="BK21" s="4"/>
     </row>
     <row r="22" spans="5:63" x14ac:dyDescent="0.25">
-      <c r="J22" s="161"/>
-      <c r="K22" s="162"/>
-      <c r="L22" s="162"/>
-      <c r="M22" s="162"/>
+      <c r="J22" s="113"/>
+      <c r="K22" s="114"/>
+      <c r="L22" s="114"/>
+      <c r="M22" s="114"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -5174,15 +5180,15 @@
       <c r="BI22" s="4"/>
     </row>
     <row r="23" spans="5:63" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J23" s="161"/>
-      <c r="K23" s="162"/>
-      <c r="L23" s="162"/>
-      <c r="M23" s="162"/>
-      <c r="N23" s="139"/>
-      <c r="O23" s="139"/>
-      <c r="P23" s="139"/>
-      <c r="Q23" s="139"/>
-      <c r="R23" s="139"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="114"/>
+      <c r="L23" s="114"/>
+      <c r="M23" s="114"/>
+      <c r="N23" s="130"/>
+      <c r="O23" s="130"/>
+      <c r="P23" s="130"/>
+      <c r="Q23" s="130"/>
+      <c r="R23" s="130"/>
       <c r="S23" s="78">
         <v>0</v>
       </c>
@@ -5259,33 +5265,33 @@
       <c r="BH23" s="79"/>
     </row>
     <row r="24" spans="5:63" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J24" s="161"/>
-      <c r="K24" s="162"/>
-      <c r="L24" s="162"/>
-      <c r="M24" s="162"/>
-      <c r="N24" s="141" t="s">
+      <c r="J24" s="113"/>
+      <c r="K24" s="114"/>
+      <c r="L24" s="114"/>
+      <c r="M24" s="114"/>
+      <c r="N24" s="164" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="141"/>
-      <c r="P24" s="141"/>
-      <c r="Q24" s="141"/>
-      <c r="R24" s="141"/>
-      <c r="S24" s="135" t="s">
+      <c r="O24" s="164"/>
+      <c r="P24" s="164"/>
+      <c r="Q24" s="164"/>
+      <c r="R24" s="164"/>
+      <c r="S24" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="T24" s="136"/>
+      <c r="T24" s="133"/>
       <c r="U24" s="85" t="s">
         <v>156</v>
       </c>
       <c r="V24" s="84" t="s">
         <v>231</v>
       </c>
-      <c r="W24" s="130" t="s">
+      <c r="W24" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="X24" s="131"/>
-      <c r="Y24" s="131"/>
-      <c r="Z24" s="132"/>
+      <c r="X24" s="128"/>
+      <c r="Y24" s="128"/>
+      <c r="Z24" s="135"/>
       <c r="AA24" s="101" t="s">
         <v>268</v>
       </c>
@@ -5306,10 +5312,10 @@
       <c r="AN24" s="4"/>
       <c r="AO24" s="4"/>
       <c r="AS24" s="25"/>
-      <c r="AX24" s="122" t="s">
+      <c r="AX24" s="154" t="s">
         <v>145</v>
       </c>
-      <c r="AY24" s="123"/>
+      <c r="AY24" s="155"/>
       <c r="AZ24" s="13" t="s">
         <v>146</v>
       </c>
@@ -5322,12 +5328,12 @@
       <c r="BC24" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="BD24" s="124" t="s">
+      <c r="BD24" s="115" t="s">
         <v>249</v>
       </c>
-      <c r="BE24" s="125"/>
-      <c r="BF24" s="125"/>
-      <c r="BG24" s="126"/>
+      <c r="BE24" s="116"/>
+      <c r="BF24" s="116"/>
+      <c r="BG24" s="117"/>
       <c r="BH24" s="29"/>
     </row>
     <row r="25" spans="5:63" x14ac:dyDescent="0.25">
@@ -5335,11 +5341,11 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="138"/>
-      <c r="O25" s="138"/>
-      <c r="P25" s="138"/>
-      <c r="Q25" s="138"/>
-      <c r="R25" s="138"/>
+      <c r="N25" s="124"/>
+      <c r="O25" s="124"/>
+      <c r="P25" s="124"/>
+      <c r="Q25" s="124"/>
+      <c r="R25" s="124"/>
       <c r="S25" s="24"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
@@ -5385,11 +5391,11 @@
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
-      <c r="N26" s="139"/>
-      <c r="O26" s="139"/>
-      <c r="P26" s="139"/>
-      <c r="Q26" s="139"/>
-      <c r="R26" s="139"/>
+      <c r="N26" s="130"/>
+      <c r="O26" s="130"/>
+      <c r="P26" s="130"/>
+      <c r="Q26" s="130"/>
+      <c r="R26" s="130"/>
       <c r="S26" s="78">
         <v>0</v>
       </c>
@@ -5457,49 +5463,49 @@
       <c r="AS26" s="79"/>
     </row>
     <row r="27" spans="5:63" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J27" s="161" t="s">
+      <c r="J27" s="113" t="s">
         <v>94</v>
       </c>
-      <c r="K27" s="162"/>
-      <c r="L27" s="162"/>
-      <c r="M27" s="162"/>
-      <c r="N27" s="137" t="s">
+      <c r="K27" s="114"/>
+      <c r="L27" s="114"/>
+      <c r="M27" s="114"/>
+      <c r="N27" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="O27" s="137"/>
-      <c r="P27" s="137"/>
-      <c r="Q27" s="137"/>
-      <c r="R27" s="137"/>
-      <c r="S27" s="135" t="s">
+      <c r="O27" s="131"/>
+      <c r="P27" s="131"/>
+      <c r="Q27" s="131"/>
+      <c r="R27" s="131"/>
+      <c r="S27" s="132" t="s">
         <v>26</v>
       </c>
-      <c r="T27" s="136"/>
-      <c r="U27" s="133">
+      <c r="T27" s="133"/>
+      <c r="U27" s="125">
         <v>0</v>
       </c>
-      <c r="V27" s="134"/>
-      <c r="W27" s="131" t="s">
+      <c r="V27" s="126"/>
+      <c r="W27" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="X27" s="131"/>
-      <c r="Y27" s="131"/>
-      <c r="Z27" s="132"/>
+      <c r="X27" s="128"/>
+      <c r="Y27" s="128"/>
+      <c r="Z27" s="135"/>
       <c r="AA27" s="118" t="s">
         <v>267</v>
       </c>
-      <c r="AB27" s="116"/>
-      <c r="AC27" s="116"/>
-      <c r="AD27" s="117"/>
+      <c r="AB27" s="119"/>
+      <c r="AC27" s="119"/>
+      <c r="AD27" s="156"/>
       <c r="AE27" s="118" t="s">
         <v>206</v>
       </c>
-      <c r="AF27" s="116"/>
-      <c r="AG27" s="116"/>
-      <c r="AH27" s="117"/>
-      <c r="AI27" s="113" t="s">
+      <c r="AF27" s="119"/>
+      <c r="AG27" s="119"/>
+      <c r="AH27" s="156"/>
+      <c r="AI27" s="165" t="s">
         <v>164</v>
       </c>
-      <c r="AJ27" s="114"/>
+      <c r="AJ27" s="166"/>
       <c r="AK27" s="48" t="s">
         <v>88</v>
       </c>
@@ -5524,15 +5530,15 @@
       <c r="BH27" s="46"/>
     </row>
     <row r="28" spans="5:63" x14ac:dyDescent="0.25">
-      <c r="J28" s="161"/>
-      <c r="K28" s="162"/>
-      <c r="L28" s="162"/>
-      <c r="M28" s="162"/>
-      <c r="N28" s="138"/>
-      <c r="O28" s="138"/>
-      <c r="P28" s="138"/>
-      <c r="Q28" s="138"/>
-      <c r="R28" s="138"/>
+      <c r="J28" s="113"/>
+      <c r="K28" s="114"/>
+      <c r="L28" s="114"/>
+      <c r="M28" s="114"/>
+      <c r="N28" s="124"/>
+      <c r="O28" s="124"/>
+      <c r="P28" s="124"/>
+      <c r="Q28" s="124"/>
+      <c r="R28" s="124"/>
       <c r="S28" s="24"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
@@ -5574,15 +5580,15 @@
     </row>
     <row r="29" spans="5:63" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="64"/>
-      <c r="J29" s="161"/>
-      <c r="K29" s="162"/>
-      <c r="L29" s="162"/>
-      <c r="M29" s="162"/>
-      <c r="N29" s="139"/>
-      <c r="O29" s="139"/>
-      <c r="P29" s="139"/>
-      <c r="Q29" s="139"/>
-      <c r="R29" s="139"/>
+      <c r="J29" s="113"/>
+      <c r="K29" s="114"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="114"/>
+      <c r="N29" s="130"/>
+      <c r="O29" s="130"/>
+      <c r="P29" s="130"/>
+      <c r="Q29" s="130"/>
+      <c r="R29" s="130"/>
       <c r="S29" s="78">
         <v>0</v>
       </c>
@@ -5661,49 +5667,49 @@
       <c r="AX29" s="65"/>
     </row>
     <row r="30" spans="5:63" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J30" s="161"/>
-      <c r="K30" s="162"/>
-      <c r="L30" s="162"/>
-      <c r="M30" s="162"/>
-      <c r="N30" s="137" t="s">
+      <c r="J30" s="113"/>
+      <c r="K30" s="114"/>
+      <c r="L30" s="114"/>
+      <c r="M30" s="114"/>
+      <c r="N30" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="O30" s="137"/>
-      <c r="P30" s="137"/>
-      <c r="Q30" s="137"/>
-      <c r="R30" s="137"/>
-      <c r="S30" s="135" t="s">
+      <c r="O30" s="131"/>
+      <c r="P30" s="131"/>
+      <c r="Q30" s="131"/>
+      <c r="R30" s="131"/>
+      <c r="S30" s="132" t="s">
         <v>26</v>
       </c>
-      <c r="T30" s="136"/>
-      <c r="U30" s="133" t="s">
+      <c r="T30" s="133"/>
+      <c r="U30" s="125" t="s">
         <v>169</v>
       </c>
-      <c r="V30" s="134"/>
-      <c r="W30" s="131" t="s">
+      <c r="V30" s="126"/>
+      <c r="W30" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="X30" s="131"/>
-      <c r="Y30" s="131"/>
-      <c r="Z30" s="132"/>
+      <c r="X30" s="128"/>
+      <c r="Y30" s="128"/>
+      <c r="Z30" s="135"/>
       <c r="AA30" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="AB30" s="116"/>
-      <c r="AC30" s="116"/>
-      <c r="AD30" s="116"/>
-      <c r="AE30" s="116"/>
-      <c r="AF30" s="116"/>
-      <c r="AG30" s="116"/>
-      <c r="AH30" s="116"/>
-      <c r="AI30" s="116"/>
-      <c r="AJ30" s="116"/>
-      <c r="AK30" s="116"/>
-      <c r="AL30" s="116"/>
-      <c r="AM30" s="116"/>
-      <c r="AN30" s="116"/>
-      <c r="AO30" s="116"/>
-      <c r="AP30" s="119"/>
+      <c r="AB30" s="119"/>
+      <c r="AC30" s="119"/>
+      <c r="AD30" s="119"/>
+      <c r="AE30" s="119"/>
+      <c r="AF30" s="119"/>
+      <c r="AG30" s="119"/>
+      <c r="AH30" s="119"/>
+      <c r="AI30" s="119"/>
+      <c r="AJ30" s="119"/>
+      <c r="AK30" s="119"/>
+      <c r="AL30" s="119"/>
+      <c r="AM30" s="119"/>
+      <c r="AN30" s="119"/>
+      <c r="AO30" s="119"/>
+      <c r="AP30" s="120"/>
       <c r="AQ30" s="2"/>
       <c r="AR30" s="4"/>
       <c r="AS30" s="25"/>
@@ -5724,11 +5730,11 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="138"/>
-      <c r="O31" s="138"/>
-      <c r="P31" s="138"/>
-      <c r="Q31" s="138"/>
-      <c r="R31" s="138"/>
+      <c r="N31" s="124"/>
+      <c r="O31" s="124"/>
+      <c r="P31" s="124"/>
+      <c r="Q31" s="124"/>
+      <c r="R31" s="124"/>
       <c r="S31" s="24"/>
       <c r="T31" s="4"/>
       <c r="U31" s="4"/>
@@ -5763,11 +5769,11 @@
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
-      <c r="N32" s="139"/>
-      <c r="O32" s="139"/>
-      <c r="P32" s="139"/>
-      <c r="Q32" s="139"/>
-      <c r="R32" s="139"/>
+      <c r="N32" s="130"/>
+      <c r="O32" s="130"/>
+      <c r="P32" s="130"/>
+      <c r="Q32" s="130"/>
+      <c r="R32" s="130"/>
       <c r="S32" s="78">
         <v>0</v>
       </c>
@@ -5813,33 +5819,33 @@
       <c r="AS32" s="79"/>
     </row>
     <row r="33" spans="8:65" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J33" s="163" t="s">
+      <c r="J33" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="K33" s="164"/>
-      <c r="L33" s="164"/>
-      <c r="M33" s="164"/>
-      <c r="N33" s="137" t="s">
+      <c r="K33" s="151"/>
+      <c r="L33" s="151"/>
+      <c r="M33" s="151"/>
+      <c r="N33" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="O33" s="137"/>
-      <c r="P33" s="137"/>
-      <c r="Q33" s="137"/>
-      <c r="R33" s="137"/>
-      <c r="S33" s="140" t="s">
+      <c r="O33" s="131"/>
+      <c r="P33" s="131"/>
+      <c r="Q33" s="131"/>
+      <c r="R33" s="131"/>
+      <c r="S33" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="T33" s="140"/>
-      <c r="U33" s="133" t="s">
+      <c r="T33" s="134"/>
+      <c r="U33" s="125" t="s">
         <v>169</v>
       </c>
-      <c r="V33" s="134"/>
-      <c r="W33" s="130" t="s">
+      <c r="V33" s="126"/>
+      <c r="W33" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="X33" s="131"/>
-      <c r="Y33" s="131"/>
-      <c r="Z33" s="170"/>
+      <c r="X33" s="128"/>
+      <c r="Y33" s="128"/>
+      <c r="Z33" s="129"/>
       <c r="AA33" s="4"/>
       <c r="AB33" s="4"/>
       <c r="AC33" s="4"/>
@@ -5861,15 +5867,15 @@
       <c r="AS33" s="25"/>
     </row>
     <row r="34" spans="8:65" x14ac:dyDescent="0.25">
-      <c r="J34" s="163"/>
-      <c r="K34" s="164"/>
-      <c r="L34" s="164"/>
-      <c r="M34" s="164"/>
-      <c r="N34" s="138"/>
-      <c r="O34" s="138"/>
-      <c r="P34" s="138"/>
-      <c r="Q34" s="138"/>
-      <c r="R34" s="138"/>
+      <c r="J34" s="150"/>
+      <c r="K34" s="151"/>
+      <c r="L34" s="151"/>
+      <c r="M34" s="151"/>
+      <c r="N34" s="124"/>
+      <c r="O34" s="124"/>
+      <c r="P34" s="124"/>
+      <c r="Q34" s="124"/>
+      <c r="R34" s="124"/>
       <c r="S34" s="24"/>
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
@@ -5899,15 +5905,15 @@
       <c r="AS34" s="25"/>
     </row>
     <row r="35" spans="8:65" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J35" s="163"/>
-      <c r="K35" s="164"/>
-      <c r="L35" s="164"/>
-      <c r="M35" s="164"/>
-      <c r="N35" s="139"/>
-      <c r="O35" s="139"/>
-      <c r="P35" s="139"/>
-      <c r="Q35" s="139"/>
-      <c r="R35" s="139"/>
+      <c r="J35" s="150"/>
+      <c r="K35" s="151"/>
+      <c r="L35" s="151"/>
+      <c r="M35" s="151"/>
+      <c r="N35" s="130"/>
+      <c r="O35" s="130"/>
+      <c r="P35" s="130"/>
+      <c r="Q35" s="130"/>
+      <c r="R35" s="130"/>
       <c r="S35" s="78">
         <v>0</v>
       </c>
@@ -5986,49 +5992,49 @@
     </row>
     <row r="36" spans="8:65" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I36" s="25"/>
-      <c r="J36" s="164"/>
-      <c r="K36" s="164"/>
-      <c r="L36" s="164"/>
-      <c r="M36" s="164"/>
-      <c r="N36" s="137" t="s">
+      <c r="J36" s="151"/>
+      <c r="K36" s="151"/>
+      <c r="L36" s="151"/>
+      <c r="M36" s="151"/>
+      <c r="N36" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="O36" s="137"/>
-      <c r="P36" s="137"/>
-      <c r="Q36" s="137"/>
-      <c r="R36" s="137"/>
-      <c r="S36" s="140" t="s">
+      <c r="O36" s="131"/>
+      <c r="P36" s="131"/>
+      <c r="Q36" s="131"/>
+      <c r="R36" s="131"/>
+      <c r="S36" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="T36" s="140"/>
-      <c r="U36" s="133" t="s">
+      <c r="T36" s="134"/>
+      <c r="U36" s="125" t="s">
         <v>169</v>
       </c>
-      <c r="V36" s="134"/>
-      <c r="W36" s="130" t="s">
+      <c r="V36" s="126"/>
+      <c r="W36" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="X36" s="131"/>
-      <c r="Y36" s="131"/>
-      <c r="Z36" s="132"/>
+      <c r="X36" s="128"/>
+      <c r="Y36" s="128"/>
+      <c r="Z36" s="135"/>
       <c r="AA36" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="AB36" s="116"/>
-      <c r="AC36" s="116"/>
-      <c r="AD36" s="116"/>
-      <c r="AE36" s="116"/>
-      <c r="AF36" s="116"/>
-      <c r="AG36" s="116"/>
-      <c r="AH36" s="116"/>
-      <c r="AI36" s="116"/>
-      <c r="AJ36" s="116"/>
-      <c r="AK36" s="116"/>
-      <c r="AL36" s="116"/>
-      <c r="AM36" s="116"/>
-      <c r="AN36" s="116"/>
-      <c r="AO36" s="116"/>
-      <c r="AP36" s="119"/>
+      <c r="AB36" s="119"/>
+      <c r="AC36" s="119"/>
+      <c r="AD36" s="119"/>
+      <c r="AE36" s="119"/>
+      <c r="AF36" s="119"/>
+      <c r="AG36" s="119"/>
+      <c r="AH36" s="119"/>
+      <c r="AI36" s="119"/>
+      <c r="AJ36" s="119"/>
+      <c r="AK36" s="119"/>
+      <c r="AL36" s="119"/>
+      <c r="AM36" s="119"/>
+      <c r="AN36" s="119"/>
+      <c r="AO36" s="119"/>
+      <c r="AP36" s="120"/>
       <c r="AQ36" s="2"/>
       <c r="AR36" s="4"/>
       <c r="AS36" s="25"/>
@@ -6108,37 +6114,37 @@
     </row>
     <row r="39" spans="8:65" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I39" s="25"/>
-      <c r="J39" s="204" t="s">
+      <c r="J39" s="139" t="s">
         <v>270</v>
       </c>
-      <c r="K39" s="204"/>
-      <c r="L39" s="204"/>
-      <c r="M39" s="204"/>
-      <c r="N39" s="137" t="s">
+      <c r="K39" s="139"/>
+      <c r="L39" s="139"/>
+      <c r="M39" s="139"/>
+      <c r="N39" s="131" t="s">
         <v>246</v>
       </c>
-      <c r="O39" s="137"/>
-      <c r="P39" s="137"/>
-      <c r="Q39" s="137"/>
-      <c r="R39" s="137"/>
-      <c r="S39" s="135" t="s">
+      <c r="O39" s="131"/>
+      <c r="P39" s="131"/>
+      <c r="Q39" s="131"/>
+      <c r="R39" s="131"/>
+      <c r="S39" s="132" t="s">
         <v>244</v>
       </c>
-      <c r="T39" s="136"/>
-      <c r="U39" s="130" t="s">
+      <c r="T39" s="133"/>
+      <c r="U39" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="V39" s="131"/>
-      <c r="W39" s="131"/>
-      <c r="X39" s="132"/>
-      <c r="Y39" s="156" t="s">
+      <c r="V39" s="128"/>
+      <c r="W39" s="128"/>
+      <c r="X39" s="135"/>
+      <c r="Y39" s="140" t="s">
         <v>245</v>
       </c>
-      <c r="Z39" s="157"/>
-      <c r="AA39" s="157"/>
-      <c r="AB39" s="157"/>
-      <c r="AC39" s="157"/>
-      <c r="AD39" s="158"/>
+      <c r="Z39" s="141"/>
+      <c r="AA39" s="141"/>
+      <c r="AB39" s="141"/>
+      <c r="AC39" s="141"/>
+      <c r="AD39" s="142"/>
       <c r="AE39" s="7"/>
       <c r="AF39" s="6"/>
       <c r="AG39" s="6"/>
@@ -6154,23 +6160,23 @@
       <c r="AQ39" s="46"/>
       <c r="AR39" s="46"/>
       <c r="AS39" s="25"/>
-      <c r="AY39" s="115" t="s">
+      <c r="AY39" s="167" t="s">
         <v>170</v>
       </c>
-      <c r="AZ39" s="115"/>
-      <c r="BA39" s="115"/>
-      <c r="BB39" s="115"/>
-      <c r="BC39" s="115"/>
-      <c r="BD39" s="115"/>
-      <c r="BE39" s="115"/>
-      <c r="BF39" s="115"/>
-      <c r="BG39" s="115"/>
-      <c r="BH39" s="115"/>
-      <c r="BI39" s="115"/>
-      <c r="BJ39" s="115"/>
-      <c r="BK39" s="115"/>
-      <c r="BL39" s="115"/>
-      <c r="BM39" s="115"/>
+      <c r="AZ39" s="167"/>
+      <c r="BA39" s="167"/>
+      <c r="BB39" s="167"/>
+      <c r="BC39" s="167"/>
+      <c r="BD39" s="167"/>
+      <c r="BE39" s="167"/>
+      <c r="BF39" s="167"/>
+      <c r="BG39" s="167"/>
+      <c r="BH39" s="167"/>
+      <c r="BI39" s="167"/>
+      <c r="BJ39" s="167"/>
+      <c r="BK39" s="167"/>
+      <c r="BL39" s="167"/>
+      <c r="BM39" s="167"/>
     </row>
     <row r="40" spans="8:65" x14ac:dyDescent="0.25">
       <c r="I40" s="25"/>
@@ -7219,6 +7225,72 @@
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="AI27:AJ27"/>
+    <mergeCell ref="AY39:BM39"/>
+    <mergeCell ref="AA18:AD18"/>
+    <mergeCell ref="AE18:AF18"/>
+    <mergeCell ref="AG18:AJ18"/>
+    <mergeCell ref="AA21:AB21"/>
+    <mergeCell ref="AE27:AH27"/>
+    <mergeCell ref="AX24:AY24"/>
+    <mergeCell ref="BD24:BG24"/>
+    <mergeCell ref="AZ21:BB21"/>
+    <mergeCell ref="W18:Z18"/>
+    <mergeCell ref="W36:Z36"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="W30:Z30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="W27:Z27"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="N36:R36"/>
+    <mergeCell ref="N25:R25"/>
+    <mergeCell ref="N26:R26"/>
+    <mergeCell ref="N33:R33"/>
+    <mergeCell ref="N34:R34"/>
+    <mergeCell ref="N32:R32"/>
+    <mergeCell ref="N27:R27"/>
+    <mergeCell ref="N28:R28"/>
+    <mergeCell ref="N29:R29"/>
+    <mergeCell ref="N30:R30"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="N18:R18"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="N35:R35"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="AT12:AV12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="U12:AS12"/>
+    <mergeCell ref="N15:R15"/>
+    <mergeCell ref="AE15:AH15"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="Y15:AB15"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:AS4"/>
+    <mergeCell ref="AY3:BF3"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="N39:R39"/>
+    <mergeCell ref="S39:T39"/>
+    <mergeCell ref="U39:X39"/>
+    <mergeCell ref="Y39:AD39"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="U8:AS8"/>
+    <mergeCell ref="AT8:AV8"/>
+    <mergeCell ref="J27:M30"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J33:M36"/>
+    <mergeCell ref="AX18:AY18"/>
+    <mergeCell ref="AX21:AY21"/>
+    <mergeCell ref="AA27:AD27"/>
     <mergeCell ref="J18:M24"/>
     <mergeCell ref="BE21:BG21"/>
     <mergeCell ref="AA36:AP36"/>
@@ -7235,72 +7307,6 @@
     <mergeCell ref="S30:T30"/>
     <mergeCell ref="W21:Z21"/>
     <mergeCell ref="W24:Z24"/>
-    <mergeCell ref="AY3:BF3"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="N39:R39"/>
-    <mergeCell ref="S39:T39"/>
-    <mergeCell ref="U39:X39"/>
-    <mergeCell ref="Y39:AD39"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="U8:AS8"/>
-    <mergeCell ref="AT8:AV8"/>
-    <mergeCell ref="J27:M30"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J33:M36"/>
-    <mergeCell ref="AX18:AY18"/>
-    <mergeCell ref="AX21:AY21"/>
-    <mergeCell ref="AA27:AD27"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:AS4"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="AT12:AV12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="U12:AS12"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="AE15:AH15"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="Y15:AB15"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="N18:R18"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="N35:R35"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="N23:R23"/>
-    <mergeCell ref="N24:R24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="N36:R36"/>
-    <mergeCell ref="N25:R25"/>
-    <mergeCell ref="N26:R26"/>
-    <mergeCell ref="N33:R33"/>
-    <mergeCell ref="N34:R34"/>
-    <mergeCell ref="N32:R32"/>
-    <mergeCell ref="N27:R27"/>
-    <mergeCell ref="N28:R28"/>
-    <mergeCell ref="N29:R29"/>
-    <mergeCell ref="N30:R30"/>
-    <mergeCell ref="W18:Z18"/>
-    <mergeCell ref="W36:Z36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="W30:Z30"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="W27:Z27"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="AI27:AJ27"/>
-    <mergeCell ref="AY39:BM39"/>
-    <mergeCell ref="AA18:AD18"/>
-    <mergeCell ref="AE18:AF18"/>
-    <mergeCell ref="AG18:AJ18"/>
-    <mergeCell ref="AA21:AB21"/>
-    <mergeCell ref="AE27:AH27"/>
-    <mergeCell ref="AX24:AY24"/>
-    <mergeCell ref="BD24:BG24"/>
-    <mergeCell ref="AZ21:BB21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="36" orientation="portrait" r:id="rId1"/>
@@ -7310,10 +7316,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E6:H14"/>
+  <dimension ref="E6:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7384,25 +7390,36 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>260</v>
-      </c>
-      <c r="F13" t="s">
-        <v>261</v>
-      </c>
-      <c r="G13" t="s">
-        <v>256</v>
+    <row r="13" spans="5:8" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="46" t="s">
+        <v>271</v>
+      </c>
+      <c r="F13" s="46">
+        <v>1</v>
+      </c>
+      <c r="H13" s="46" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" t="s">
+        <v>261</v>
+      </c>
+      <c r="G14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>264</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>247</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>266</v>
       </c>
     </row>
@@ -8071,12 +8088,12 @@
       <c r="B5" s="56">
         <v>4</v>
       </c>
-      <c r="C5" s="171" t="s">
+      <c r="C5" s="185" t="s">
         <v>214</v>
       </c>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="173"/>
+      <c r="D5" s="186"/>
+      <c r="E5" s="186"/>
+      <c r="F5" s="187"/>
       <c r="G5" s="63"/>
       <c r="H5" s="49" t="s">
         <v>225</v>
@@ -8084,169 +8101,169 @@
       <c r="I5" s="67">
         <v>0</v>
       </c>
-      <c r="J5" s="185" t="s">
+      <c r="J5" s="197" t="s">
         <v>239</v>
       </c>
-      <c r="K5" s="186"/>
-      <c r="L5" s="177" t="s">
+      <c r="K5" s="198"/>
+      <c r="L5" s="191" t="s">
         <v>156</v>
       </c>
-      <c r="M5" s="178"/>
+      <c r="M5" s="192"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="56">
         <v>8</v>
       </c>
-      <c r="C6" s="174"/>
-      <c r="D6" s="175"/>
-      <c r="E6" s="175"/>
-      <c r="F6" s="176"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="190"/>
       <c r="G6" s="63"/>
       <c r="I6" s="68">
         <v>4</v>
       </c>
-      <c r="J6" s="179" t="s">
+      <c r="J6" s="176" t="s">
         <v>216</v>
       </c>
-      <c r="K6" s="179"/>
-      <c r="L6" s="179"/>
-      <c r="M6" s="180"/>
+      <c r="K6" s="176"/>
+      <c r="L6" s="176"/>
+      <c r="M6" s="177"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="56">
         <v>12</v>
       </c>
-      <c r="C7" s="174"/>
-      <c r="D7" s="175"/>
-      <c r="E7" s="175"/>
-      <c r="F7" s="176"/>
+      <c r="C7" s="188"/>
+      <c r="D7" s="189"/>
+      <c r="E7" s="189"/>
+      <c r="F7" s="190"/>
       <c r="G7" s="63"/>
       <c r="I7" s="68">
         <v>8</v>
       </c>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="181"/>
-      <c r="M7" s="182"/>
+      <c r="J7" s="193"/>
+      <c r="K7" s="193"/>
+      <c r="L7" s="193"/>
+      <c r="M7" s="194"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="56">
         <v>16</v>
       </c>
-      <c r="C8" s="174"/>
-      <c r="D8" s="175"/>
-      <c r="E8" s="175"/>
-      <c r="F8" s="176"/>
+      <c r="C8" s="188"/>
+      <c r="D8" s="189"/>
+      <c r="E8" s="189"/>
+      <c r="F8" s="190"/>
       <c r="G8" s="63"/>
       <c r="I8" s="68">
         <v>12</v>
       </c>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="181"/>
-      <c r="M8" s="182"/>
+      <c r="J8" s="193"/>
+      <c r="K8" s="193"/>
+      <c r="L8" s="193"/>
+      <c r="M8" s="194"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="56">
         <v>20</v>
       </c>
-      <c r="C9" s="174"/>
-      <c r="D9" s="175"/>
-      <c r="E9" s="175"/>
-      <c r="F9" s="176"/>
+      <c r="C9" s="188"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="190"/>
       <c r="G9" s="63"/>
       <c r="I9" s="68">
         <v>16</v>
       </c>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="181"/>
-      <c r="M9" s="182"/>
+      <c r="J9" s="193"/>
+      <c r="K9" s="193"/>
+      <c r="L9" s="193"/>
+      <c r="M9" s="194"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="56">
         <v>24</v>
       </c>
-      <c r="C10" s="174"/>
-      <c r="D10" s="175"/>
-      <c r="E10" s="175"/>
-      <c r="F10" s="176"/>
+      <c r="C10" s="188"/>
+      <c r="D10" s="189"/>
+      <c r="E10" s="189"/>
+      <c r="F10" s="190"/>
       <c r="G10" s="63"/>
       <c r="I10" s="68">
         <v>20</v>
       </c>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="181"/>
-      <c r="M10" s="182"/>
+      <c r="J10" s="193"/>
+      <c r="K10" s="193"/>
+      <c r="L10" s="193"/>
+      <c r="M10" s="194"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="56">
         <v>28</v>
       </c>
-      <c r="C11" s="174"/>
-      <c r="D11" s="175"/>
-      <c r="E11" s="175"/>
-      <c r="F11" s="176"/>
+      <c r="C11" s="188"/>
+      <c r="D11" s="189"/>
+      <c r="E11" s="189"/>
+      <c r="F11" s="190"/>
       <c r="G11" s="63"/>
       <c r="I11" s="68">
         <v>24</v>
       </c>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="181"/>
-      <c r="M11" s="182"/>
+      <c r="J11" s="193"/>
+      <c r="K11" s="193"/>
+      <c r="L11" s="193"/>
+      <c r="M11" s="194"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="56">
         <v>32</v>
       </c>
-      <c r="C12" s="174"/>
-      <c r="D12" s="175"/>
-      <c r="E12" s="175"/>
-      <c r="F12" s="176"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="189"/>
+      <c r="E12" s="189"/>
+      <c r="F12" s="190"/>
       <c r="G12" s="63"/>
       <c r="I12" s="68">
         <v>28</v>
       </c>
-      <c r="J12" s="181"/>
-      <c r="K12" s="181"/>
-      <c r="L12" s="181"/>
-      <c r="M12" s="182"/>
+      <c r="J12" s="193"/>
+      <c r="K12" s="193"/>
+      <c r="L12" s="193"/>
+      <c r="M12" s="194"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="56">
         <v>36</v>
       </c>
-      <c r="C13" s="174"/>
-      <c r="D13" s="175"/>
-      <c r="E13" s="175"/>
-      <c r="F13" s="176"/>
+      <c r="C13" s="188"/>
+      <c r="D13" s="189"/>
+      <c r="E13" s="189"/>
+      <c r="F13" s="190"/>
       <c r="G13" s="63"/>
       <c r="I13" s="68">
         <v>32</v>
       </c>
-      <c r="J13" s="181"/>
-      <c r="K13" s="181"/>
-      <c r="L13" s="181"/>
-      <c r="M13" s="182"/>
+      <c r="J13" s="193"/>
+      <c r="K13" s="193"/>
+      <c r="L13" s="193"/>
+      <c r="M13" s="194"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="56">
         <v>40</v>
       </c>
-      <c r="C14" s="174"/>
-      <c r="D14" s="175"/>
-      <c r="E14" s="175"/>
-      <c r="F14" s="176"/>
+      <c r="C14" s="188"/>
+      <c r="D14" s="189"/>
+      <c r="E14" s="189"/>
+      <c r="F14" s="190"/>
       <c r="G14" s="63"/>
       <c r="I14" s="68">
         <v>36</v>
       </c>
-      <c r="J14" s="181"/>
-      <c r="K14" s="181"/>
-      <c r="L14" s="181"/>
-      <c r="M14" s="182"/>
+      <c r="J14" s="193"/>
+      <c r="K14" s="193"/>
+      <c r="L14" s="193"/>
+      <c r="M14" s="194"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="56">
@@ -8260,10 +8277,10 @@
       <c r="I15" s="68">
         <v>40</v>
       </c>
-      <c r="J15" s="181"/>
-      <c r="K15" s="181"/>
-      <c r="L15" s="181"/>
-      <c r="M15" s="182"/>
+      <c r="J15" s="193"/>
+      <c r="K15" s="193"/>
+      <c r="L15" s="193"/>
+      <c r="M15" s="194"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="62" t="s">
@@ -8277,10 +8294,10 @@
       <c r="I16" s="68">
         <v>44</v>
       </c>
-      <c r="J16" s="181"/>
-      <c r="K16" s="181"/>
-      <c r="L16" s="181"/>
-      <c r="M16" s="182"/>
+      <c r="J16" s="193"/>
+      <c r="K16" s="193"/>
+      <c r="L16" s="193"/>
+      <c r="M16" s="194"/>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="62" t="s">
@@ -8294,9 +8311,9 @@
       <c r="I17" s="68">
         <v>48</v>
       </c>
-      <c r="J17" s="181"/>
-      <c r="K17" s="181"/>
-      <c r="L17" s="181"/>
+      <c r="J17" s="193"/>
+      <c r="K17" s="193"/>
+      <c r="L17" s="193"/>
       <c r="M17" s="66"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -8314,14 +8331,14 @@
       <c r="I18" s="67">
         <v>52</v>
       </c>
-      <c r="J18" s="185">
+      <c r="J18" s="197">
         <v>8</v>
       </c>
-      <c r="K18" s="186"/>
-      <c r="L18" s="177" t="s">
+      <c r="K18" s="198"/>
+      <c r="L18" s="191" t="s">
         <v>217</v>
       </c>
-      <c r="M18" s="178"/>
+      <c r="M18" s="192"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="61"/>
@@ -8333,12 +8350,12 @@
       <c r="I19" s="68">
         <v>56</v>
       </c>
-      <c r="J19" s="179" t="s">
+      <c r="J19" s="176" t="s">
         <v>218</v>
       </c>
-      <c r="K19" s="179"/>
-      <c r="L19" s="179"/>
-      <c r="M19" s="180"/>
+      <c r="K19" s="176"/>
+      <c r="L19" s="176"/>
+      <c r="M19" s="177"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="61"/>
@@ -8350,10 +8367,10 @@
       <c r="I20" s="68">
         <v>60</v>
       </c>
-      <c r="J20" s="181"/>
-      <c r="K20" s="181"/>
-      <c r="L20" s="181"/>
-      <c r="M20" s="182"/>
+      <c r="J20" s="193"/>
+      <c r="K20" s="193"/>
+      <c r="L20" s="193"/>
+      <c r="M20" s="194"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="61"/>
@@ -8365,10 +8382,10 @@
       <c r="I21" s="68">
         <v>64</v>
       </c>
-      <c r="J21" s="181"/>
-      <c r="K21" s="181"/>
-      <c r="L21" s="181"/>
-      <c r="M21" s="182"/>
+      <c r="J21" s="193"/>
+      <c r="K21" s="193"/>
+      <c r="L21" s="193"/>
+      <c r="M21" s="194"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="61"/>
@@ -8380,10 +8397,10 @@
       <c r="I22" s="68">
         <v>68</v>
       </c>
-      <c r="J22" s="181"/>
-      <c r="K22" s="181"/>
-      <c r="L22" s="181"/>
-      <c r="M22" s="182"/>
+      <c r="J22" s="193"/>
+      <c r="K22" s="193"/>
+      <c r="L22" s="193"/>
+      <c r="M22" s="194"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="44"/>
@@ -8395,10 +8412,10 @@
       <c r="I23" s="68">
         <v>72</v>
       </c>
-      <c r="J23" s="181"/>
-      <c r="K23" s="181"/>
-      <c r="L23" s="181"/>
-      <c r="M23" s="182"/>
+      <c r="J23" s="193"/>
+      <c r="K23" s="193"/>
+      <c r="L23" s="193"/>
+      <c r="M23" s="194"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="44"/>
@@ -8410,10 +8427,10 @@
       <c r="I24" s="68">
         <v>76</v>
       </c>
-      <c r="J24" s="181"/>
-      <c r="K24" s="181"/>
-      <c r="L24" s="181"/>
-      <c r="M24" s="182"/>
+      <c r="J24" s="193"/>
+      <c r="K24" s="193"/>
+      <c r="L24" s="193"/>
+      <c r="M24" s="194"/>
     </row>
     <row r="25" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="44"/>
@@ -8425,10 +8442,10 @@
       <c r="I25" s="69">
         <v>80</v>
       </c>
-      <c r="J25" s="183"/>
-      <c r="K25" s="183"/>
-      <c r="L25" s="183"/>
-      <c r="M25" s="184"/>
+      <c r="J25" s="195"/>
+      <c r="K25" s="195"/>
+      <c r="L25" s="195"/>
+      <c r="M25" s="196"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="44"/>
@@ -8443,14 +8460,14 @@
       <c r="I26" s="68">
         <v>84</v>
       </c>
-      <c r="J26" s="185">
+      <c r="J26" s="197">
         <v>8</v>
       </c>
-      <c r="K26" s="186"/>
-      <c r="L26" s="177" t="s">
+      <c r="K26" s="198"/>
+      <c r="L26" s="191" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="178"/>
+      <c r="M26" s="192"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="44"/>
@@ -8462,14 +8479,14 @@
       <c r="I27" s="68">
         <v>88</v>
       </c>
-      <c r="J27" s="187" t="s">
+      <c r="J27" s="172" t="s">
         <v>219</v>
       </c>
-      <c r="K27" s="188"/>
-      <c r="L27" s="189" t="s">
+      <c r="K27" s="173"/>
+      <c r="L27" s="174" t="s">
         <v>220</v>
       </c>
-      <c r="M27" s="190"/>
+      <c r="M27" s="175"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="44"/>
@@ -8481,12 +8498,12 @@
       <c r="I28" s="68">
         <v>92</v>
       </c>
-      <c r="J28" s="179" t="s">
+      <c r="J28" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="K28" s="179"/>
-      <c r="L28" s="179"/>
-      <c r="M28" s="180"/>
+      <c r="K28" s="176"/>
+      <c r="L28" s="176"/>
+      <c r="M28" s="177"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="44"/>
@@ -8498,12 +8515,12 @@
       <c r="I29" s="68">
         <v>96</v>
       </c>
-      <c r="J29" s="187" t="s">
+      <c r="J29" s="172" t="s">
         <v>10</v>
       </c>
-      <c r="K29" s="187"/>
-      <c r="L29" s="187"/>
-      <c r="M29" s="190"/>
+      <c r="K29" s="172"/>
+      <c r="L29" s="172"/>
+      <c r="M29" s="175"/>
     </row>
     <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="44"/>
@@ -8515,12 +8532,12 @@
       <c r="I30" s="68">
         <v>100</v>
       </c>
-      <c r="J30" s="179" t="s">
+      <c r="J30" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="K30" s="191"/>
-      <c r="L30" s="194"/>
-      <c r="M30" s="195"/>
+      <c r="K30" s="178"/>
+      <c r="L30" s="181"/>
+      <c r="M30" s="182"/>
     </row>
     <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="44"/>
@@ -8535,14 +8552,14 @@
       <c r="I31" s="83">
         <v>104</v>
       </c>
-      <c r="J31" s="196" t="s">
+      <c r="J31" s="183" t="s">
         <v>240</v>
       </c>
-      <c r="K31" s="197"/>
-      <c r="L31" s="192" t="s">
+      <c r="K31" s="184"/>
+      <c r="L31" s="179" t="s">
         <v>222</v>
       </c>
-      <c r="M31" s="193"/>
+      <c r="M31" s="180"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="44"/>
@@ -8565,10 +8582,10 @@
       <c r="F33" s="58"/>
       <c r="G33" s="58"/>
       <c r="I33" s="61"/>
-      <c r="J33" s="153" t="s">
+      <c r="J33" s="136" t="s">
         <v>243</v>
       </c>
-      <c r="K33" s="155"/>
+      <c r="K33" s="138"/>
       <c r="L33" s="58"/>
       <c r="M33" s="58"/>
       <c r="N33" s="11"/>
@@ -8612,15 +8629,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
     <mergeCell ref="C5:F14"/>
     <mergeCell ref="L26:M26"/>
     <mergeCell ref="J19:M25"/>
@@ -8631,6 +8639,15 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8683,7 +8700,7 @@
       </c>
     </row>
     <row r="5" spans="3:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="198" t="s">
+      <c r="C5" s="199" t="s">
         <v>200</v>
       </c>
       <c r="D5" s="37" t="s">
@@ -8701,7 +8718,7 @@
       </c>
     </row>
     <row r="6" spans="3:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="198"/>
+      <c r="C6" s="199"/>
       <c r="D6" s="38" t="s">
         <v>194</v>
       </c>
@@ -8717,7 +8734,7 @@
       </c>
     </row>
     <row r="7" spans="3:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="198"/>
+      <c r="C7" s="199"/>
       <c r="D7" s="38" t="s">
         <v>197</v>
       </c>
@@ -8733,7 +8750,7 @@
       </c>
     </row>
     <row r="8" spans="3:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="198"/>
+      <c r="C8" s="199"/>
       <c r="D8" s="38" t="s">
         <v>198</v>
       </c>
@@ -8749,7 +8766,7 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="198"/>
+      <c r="C9" s="199"/>
       <c r="D9" s="38" t="s">
         <v>187</v>
       </c>
@@ -8765,7 +8782,7 @@
       </c>
     </row>
     <row r="10" spans="3:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="198"/>
+      <c r="C10" s="199"/>
       <c r="D10" s="38" t="s">
         <v>195</v>
       </c>
@@ -8781,7 +8798,7 @@
       </c>
     </row>
     <row r="11" spans="3:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="198"/>
+      <c r="C11" s="199"/>
       <c r="D11" s="38" t="s">
         <v>192</v>
       </c>
@@ -8797,7 +8814,7 @@
       </c>
     </row>
     <row r="12" spans="3:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="198"/>
+      <c r="C12" s="199"/>
       <c r="D12" s="38" t="s">
         <v>196</v>
       </c>
@@ -8828,7 +8845,7 @@
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="198" t="s">
+      <c r="C14" s="199" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="37" t="s">
@@ -8843,7 +8860,7 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="198"/>
+      <c r="C15" s="199"/>
       <c r="D15" s="38" t="s">
         <v>167</v>
       </c>
@@ -8856,7 +8873,7 @@
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="198"/>
+      <c r="C16" s="199"/>
       <c r="D16" s="38" t="s">
         <v>12</v>
       </c>
@@ -8869,7 +8886,7 @@
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="198"/>
+      <c r="C17" s="199"/>
       <c r="D17" s="38" t="s">
         <v>11</v>
       </c>
@@ -8882,7 +8899,7 @@
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="198"/>
+      <c r="C18" s="199"/>
       <c r="D18" s="38" t="s">
         <v>168</v>
       </c>
@@ -8895,7 +8912,7 @@
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="198"/>
+      <c r="C19" s="199"/>
       <c r="D19" s="39" t="s">
         <v>10</v>
       </c>
@@ -9164,56 +9181,56 @@
   <sheetData>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="200" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="199"/>
-      <c r="D4" s="199"/>
-      <c r="E4" s="199"/>
+      <c r="C4" s="200"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="200"/>
     </row>
     <row r="5" spans="2:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="203" t="s">
+      <c r="B5" s="204" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="203"/>
-      <c r="D5" s="203" t="s">
+      <c r="C5" s="204"/>
+      <c r="D5" s="204" t="s">
         <v>151</v>
       </c>
-      <c r="E5" s="203"/>
+      <c r="E5" s="204"/>
     </row>
     <row r="6" spans="2:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="203" t="s">
+      <c r="B6" s="204" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="203"/>
-      <c r="D6" s="203"/>
-      <c r="E6" s="203"/>
+      <c r="C6" s="204"/>
+      <c r="D6" s="204"/>
+      <c r="E6" s="204"/>
     </row>
     <row r="7" spans="2:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="202" t="s">
+      <c r="B7" s="203" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="202"/>
-      <c r="D7" s="202"/>
-      <c r="E7" s="202"/>
+      <c r="C7" s="203"/>
+      <c r="D7" s="203"/>
+      <c r="E7" s="203"/>
     </row>
     <row r="8" spans="2:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="201" t="s">
+      <c r="B8" s="202" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="201"/>
-      <c r="D8" s="201" t="s">
+      <c r="C8" s="202"/>
+      <c r="D8" s="202" t="s">
         <v>148</v>
       </c>
-      <c r="E8" s="201"/>
+      <c r="E8" s="202"/>
     </row>
     <row r="9" spans="2:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="200" t="s">
+      <c r="B9" s="201" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="200"/>
-      <c r="D9" s="200"/>
-      <c r="E9" s="200"/>
+      <c r="C9" s="201"/>
+      <c r="D9" s="201"/>
+      <c r="E9" s="201"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>